<commit_message>
preliminary conference schedule (plus fixes in tourism page)
</commit_message>
<xml_diff>
--- a/docs/schedule_2016.xlsx
+++ b/docs/schedule_2016.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="0" windowWidth="18825" windowHeight="14865" tabRatio="500"/>
+    <workbookView xWindow="7800" yWindow="0" windowWidth="18825" windowHeight="14865" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="62">
   <si>
     <t>Day</t>
   </si>
@@ -223,6 +223,12 @@
   <si>
     <t>Enabling Research in Future Wireless and Mobile Networks
 (Esmeralda 1)</t>
+  </si>
+  <si>
+    <t>Printing</t>
+  </si>
+  <si>
+    <t>200x590</t>
   </si>
 </sst>
 </file>
@@ -1763,7 +1769,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1801,12 +1807,171 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="20" fontId="9" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="20" fontId="9" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="8" borderId="15" xfId="59" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="8" borderId="16" xfId="59" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="8" borderId="17" xfId="59" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1834,168 +1999,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="8" borderId="15" xfId="59" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="8" borderId="16" xfId="59" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="8" borderId="17" xfId="59" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="762">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
@@ -3100,8 +3107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E13"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
@@ -3122,31 +3129,31 @@
       <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="59" t="s">
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="60"/>
-      <c r="H2" s="49" t="s">
+      <c r="G2" s="68"/>
+      <c r="H2" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="50"/>
-      <c r="J2" s="61" t="s">
+      <c r="I2" s="58"/>
+      <c r="J2" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="59" t="s">
+      <c r="K2" s="59"/>
+      <c r="L2" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="67"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="38"/>
       <c r="Q2" s="15" t="s">
         <v>0</v>
       </c>
@@ -3167,14 +3174,14 @@
       <c r="E3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="52" t="s">
+      <c r="F3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="54"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="62"/>
       <c r="L3" s="8" t="s">
         <v>43</v>
       </c>
@@ -3195,33 +3202,33 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="81" t="s">
         <v>45</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="42"/>
-      <c r="H4" s="45" t="s">
+      <c r="G4" s="51"/>
+      <c r="H4" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="46"/>
-      <c r="J4" s="45" t="s">
+      <c r="I4" s="55"/>
+      <c r="J4" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="K4" s="55"/>
+      <c r="K4" s="63"/>
       <c r="L4" s="33" t="s">
         <v>47</v>
       </c>
@@ -3231,283 +3238,283 @@
       <c r="N4" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="O4" s="34" t="s">
+      <c r="O4" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="68" t="s">
+      <c r="P4" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="Q4" s="17" t="s">
+      <c r="Q4" s="39" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1">
-      <c r="A5" s="17"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="17"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="39"/>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1">
-      <c r="A6" s="17"/>
-      <c r="B6" s="28" t="s">
+      <c r="A6" s="39"/>
+      <c r="B6" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="30" t="s">
+      <c r="F6" s="52"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="30" t="s">
+      <c r="M6" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="30" t="s">
+      <c r="N6" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="O6" s="35" t="s">
+      <c r="O6" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="P6" s="69" t="s">
+      <c r="P6" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="Q6" s="17"/>
+      <c r="Q6" s="39"/>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1">
-      <c r="A7" s="17"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="17"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="39"/>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1">
-      <c r="A8" s="17"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="17"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="39"/>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="45" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="46"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="69"/>
-      <c r="Q9" s="17"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="64"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="39"/>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="17"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="39"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1">
-      <c r="A11" s="17"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="69"/>
-      <c r="Q11" s="17"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="39"/>
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1">
-      <c r="A12" s="17"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="69"/>
-      <c r="Q12" s="17"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="39"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1">
-      <c r="A13" s="17"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="70"/>
-      <c r="Q13" s="17"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="39"/>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1">
-      <c r="A14" s="17"/>
-      <c r="B14" s="19" t="s">
+      <c r="A14" s="39"/>
+      <c r="B14" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="37" t="s">
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="38"/>
-      <c r="H14" s="37" t="s">
+      <c r="G14" s="47"/>
+      <c r="H14" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="38"/>
-      <c r="J14" s="62" t="s">
+      <c r="I14" s="47"/>
+      <c r="J14" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="K14" s="62"/>
-      <c r="L14" s="64" t="s">
+      <c r="K14" s="70"/>
+      <c r="L14" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="M14" s="64"/>
-      <c r="N14" s="64"/>
-      <c r="O14" s="64"/>
-      <c r="P14" s="64"/>
-      <c r="Q14" s="17"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="39"/>
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1">
-      <c r="A15" s="17"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="63"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="64"/>
-      <c r="N15" s="64"/>
-      <c r="O15" s="64"/>
-      <c r="P15" s="64"/>
-      <c r="Q15" s="17"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="72"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="71"/>
+      <c r="K15" s="71"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="42"/>
+      <c r="N15" s="42"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="39"/>
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="81" t="s">
         <v>45</v>
       </c>
       <c r="C16" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="79" t="s">
+      <c r="F16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="79"/>
-      <c r="H16" s="79" t="s">
+      <c r="G16" s="20"/>
+      <c r="H16" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="79"/>
-      <c r="J16" s="79" t="s">
+      <c r="I16" s="20"/>
+      <c r="J16" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="K16" s="79"/>
+      <c r="K16" s="20"/>
       <c r="L16" s="33" t="s">
         <v>47</v>
       </c>
@@ -3517,349 +3524,349 @@
       <c r="N16" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="O16" s="34" t="s">
+      <c r="O16" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="P16" s="68" t="s">
+      <c r="P16" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="Q16" s="17" t="s">
+      <c r="Q16" s="39" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="15" customHeight="1">
-      <c r="A17" s="17"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="79"/>
-      <c r="G17" s="79"/>
-      <c r="H17" s="79"/>
-      <c r="I17" s="79"/>
-      <c r="J17" s="79"/>
-      <c r="K17" s="79"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="69"/>
-      <c r="Q17" s="17"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="39"/>
     </row>
     <row r="18" spans="1:17" ht="15" customHeight="1">
-      <c r="A18" s="17"/>
-      <c r="B18" s="28" t="s">
+      <c r="A18" s="39"/>
+      <c r="B18" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="79"/>
-      <c r="G18" s="79"/>
-      <c r="H18" s="79"/>
-      <c r="I18" s="79"/>
-      <c r="J18" s="79"/>
-      <c r="K18" s="79"/>
-      <c r="L18" s="28" t="s">
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="M18" s="30" t="s">
+      <c r="M18" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="N18" s="30" t="s">
+      <c r="N18" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="O18" s="35" t="s">
+      <c r="O18" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="P18" s="69" t="s">
+      <c r="P18" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="Q18" s="17"/>
+      <c r="Q18" s="39"/>
     </row>
     <row r="19" spans="1:17" ht="15" customHeight="1">
-      <c r="A19" s="17"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="79"/>
-      <c r="J19" s="79"/>
-      <c r="K19" s="79"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="69"/>
-      <c r="Q19" s="17"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="39"/>
     </row>
     <row r="20" spans="1:17" ht="15" customHeight="1">
-      <c r="A20" s="17"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="79"/>
-      <c r="G20" s="79"/>
-      <c r="H20" s="79"/>
-      <c r="I20" s="79"/>
-      <c r="J20" s="79"/>
-      <c r="K20" s="79"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="35"/>
-      <c r="P20" s="69"/>
-      <c r="Q20" s="17"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="39"/>
     </row>
     <row r="21" spans="1:17" ht="15" customHeight="1">
-      <c r="A21" s="17"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="79"/>
-      <c r="G21" s="79"/>
-      <c r="H21" s="79"/>
-      <c r="I21" s="79"/>
-      <c r="J21" s="79"/>
-      <c r="K21" s="79"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="35"/>
-      <c r="P21" s="69"/>
-      <c r="Q21" s="17"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="39"/>
     </row>
     <row r="22" spans="1:17" ht="15" customHeight="1">
-      <c r="A22" s="17"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="79"/>
-      <c r="G22" s="79"/>
-      <c r="H22" s="79"/>
-      <c r="I22" s="79"/>
-      <c r="J22" s="79"/>
-      <c r="K22" s="79"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="35"/>
-      <c r="P22" s="69"/>
-      <c r="Q22" s="17"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="39"/>
     </row>
     <row r="23" spans="1:17" ht="15" customHeight="1">
-      <c r="A23" s="17"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="79"/>
-      <c r="H23" s="79"/>
-      <c r="I23" s="79"/>
-      <c r="J23" s="79"/>
-      <c r="K23" s="79"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="69"/>
-      <c r="Q23" s="17"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="39"/>
     </row>
     <row r="24" spans="1:17" ht="15" customHeight="1">
-      <c r="A24" s="17"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="79"/>
-      <c r="J24" s="79"/>
-      <c r="K24" s="79"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="35"/>
-      <c r="P24" s="69"/>
-      <c r="Q24" s="17"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="39"/>
     </row>
     <row r="25" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A25" s="17"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="79"/>
-      <c r="G25" s="79"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="79"/>
-      <c r="J25" s="79"/>
-      <c r="K25" s="79"/>
-      <c r="L25" s="66"/>
-      <c r="M25" s="65"/>
-      <c r="N25" s="65"/>
-      <c r="O25" s="80"/>
-      <c r="P25" s="81"/>
-      <c r="Q25" s="17"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="39"/>
     </row>
     <row r="26" spans="1:17" ht="15" customHeight="1" thickTop="1">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="71" t="s">
+      <c r="C26" s="76"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G26" s="71"/>
-      <c r="H26" s="73" t="s">
+      <c r="G26" s="21"/>
+      <c r="H26" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="I26" s="73"/>
-      <c r="J26" s="71" t="s">
+      <c r="I26" s="23"/>
+      <c r="J26" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="71"/>
-      <c r="L26" s="75"/>
-      <c r="M26" s="76"/>
-      <c r="N26" s="76"/>
-      <c r="O26" s="76"/>
-      <c r="P26" s="77"/>
-      <c r="Q26" s="17" t="s">
+      <c r="K26" s="21"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="39" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="15" customHeight="1">
-      <c r="A27" s="17"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="73"/>
-      <c r="I27" s="73"/>
-      <c r="J27" s="71"/>
-      <c r="K27" s="71"/>
-      <c r="L27" s="75"/>
-      <c r="M27" s="78"/>
-      <c r="N27" s="78"/>
-      <c r="O27" s="78"/>
-      <c r="P27" s="77"/>
-      <c r="Q27" s="17"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="28"/>
+      <c r="P27" s="27"/>
+      <c r="Q27" s="39"/>
     </row>
     <row r="28" spans="1:17" ht="15" customHeight="1">
-      <c r="A28" s="17"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="73"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="71"/>
-      <c r="L28" s="75"/>
-      <c r="M28" s="78"/>
-      <c r="N28" s="78"/>
-      <c r="O28" s="78"/>
-      <c r="P28" s="77"/>
-      <c r="Q28" s="17"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="77"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="27"/>
+      <c r="Q28" s="39"/>
     </row>
     <row r="29" spans="1:17" ht="15" customHeight="1">
-      <c r="A29" s="17"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="71"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="73"/>
-      <c r="I29" s="73"/>
-      <c r="J29" s="71"/>
-      <c r="K29" s="71"/>
-      <c r="L29" s="75"/>
-      <c r="M29" s="78"/>
-      <c r="N29" s="78"/>
-      <c r="O29" s="78"/>
-      <c r="P29" s="77"/>
-      <c r="Q29" s="17"/>
+      <c r="A29" s="39"/>
+      <c r="B29" s="75"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="39"/>
     </row>
     <row r="30" spans="1:17" ht="15" customHeight="1">
-      <c r="A30" s="17"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="73"/>
-      <c r="I30" s="73"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="71"/>
-      <c r="L30" s="75"/>
-      <c r="M30" s="78"/>
-      <c r="N30" s="78"/>
-      <c r="O30" s="78"/>
-      <c r="P30" s="77"/>
-      <c r="Q30" s="17"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="27"/>
+      <c r="Q30" s="39"/>
     </row>
     <row r="31" spans="1:17" ht="15" customHeight="1">
-      <c r="A31" s="17"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="73"/>
-      <c r="I31" s="73"/>
-      <c r="J31" s="71"/>
-      <c r="K31" s="71"/>
-      <c r="L31" s="75"/>
-      <c r="M31" s="78"/>
-      <c r="N31" s="78"/>
-      <c r="O31" s="78"/>
-      <c r="P31" s="77"/>
-      <c r="Q31" s="17"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="28"/>
+      <c r="N31" s="28"/>
+      <c r="O31" s="28"/>
+      <c r="P31" s="27"/>
+      <c r="Q31" s="39"/>
     </row>
     <row r="32" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A32" s="18"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="72"/>
-      <c r="H32" s="74"/>
-      <c r="I32" s="74"/>
-      <c r="J32" s="72"/>
-      <c r="K32" s="72"/>
-      <c r="L32" s="75"/>
-      <c r="M32" s="78"/>
-      <c r="N32" s="78"/>
-      <c r="O32" s="78"/>
-      <c r="P32" s="77"/>
-      <c r="Q32" s="18"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="78"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="79"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="28"/>
+      <c r="P32" s="27"/>
+      <c r="Q32" s="41"/>
     </row>
     <row r="33" spans="18:18" ht="15" customHeight="1" thickTop="1"/>
     <row r="34" spans="18:18" ht="15" customHeight="1"/>
@@ -3905,57 +3912,6 @@
     <row r="68" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E25"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D25"/>
-    <mergeCell ref="J16:K25"/>
-    <mergeCell ref="F26:G32"/>
-    <mergeCell ref="H26:I32"/>
-    <mergeCell ref="J26:K32"/>
-    <mergeCell ref="L26:P32"/>
-    <mergeCell ref="F16:G25"/>
-    <mergeCell ref="H16:I25"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="O18:O25"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="P18:P25"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="N6:N13"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="Q4:Q13"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="L6:L13"/>
-    <mergeCell ref="M6:M13"/>
-    <mergeCell ref="O6:O13"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="P6:P13"/>
-    <mergeCell ref="Q14:Q15"/>
-    <mergeCell ref="Q16:Q25"/>
-    <mergeCell ref="Q26:Q32"/>
-    <mergeCell ref="L14:P15"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="N18:N25"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="L18:L25"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="M18:M25"/>
-    <mergeCell ref="F14:G15"/>
-    <mergeCell ref="F4:G8"/>
-    <mergeCell ref="F9:G13"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F3:K3"/>
-    <mergeCell ref="H4:I13"/>
-    <mergeCell ref="J4:K13"/>
-    <mergeCell ref="B6:B13"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J14:K15"/>
-    <mergeCell ref="H14:I15"/>
-    <mergeCell ref="E6:E13"/>
     <mergeCell ref="A4:A13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A25"/>
@@ -3972,11 +3928,62 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="D6:D13"/>
     <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F14:G15"/>
+    <mergeCell ref="F4:G8"/>
+    <mergeCell ref="F9:G13"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F3:K3"/>
+    <mergeCell ref="H4:I13"/>
+    <mergeCell ref="J4:K13"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J14:K15"/>
+    <mergeCell ref="H14:I15"/>
+    <mergeCell ref="E6:E13"/>
+    <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="Q16:Q25"/>
+    <mergeCell ref="Q26:Q32"/>
+    <mergeCell ref="L14:P15"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="N18:N25"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="L18:L25"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="M18:M25"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="N6:N13"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="Q4:Q13"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="L6:L13"/>
+    <mergeCell ref="M6:M13"/>
+    <mergeCell ref="O6:O13"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="P6:P13"/>
+    <mergeCell ref="F26:G32"/>
+    <mergeCell ref="H26:I32"/>
+    <mergeCell ref="J26:K32"/>
+    <mergeCell ref="L26:P32"/>
+    <mergeCell ref="F16:G25"/>
+    <mergeCell ref="H16:I25"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="O18:O25"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="P18:P25"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E25"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D25"/>
+    <mergeCell ref="J16:K25"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
-  <pageSetup paperSize="32767" scale="33" orientation="portrait" horizontalDpi="4000" verticalDpi="4000" r:id="rId1"/>
+  <pageSetup paperSize="32767" scale="95" orientation="landscape" horizontalDpi="4000" verticalDpi="4000" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="20"/>
@@ -3989,8 +3996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4265,9 +4272,15 @@
       <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
+      <c r="A32" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="82">
+        <v>0.95</v>
+      </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
     </row>

</xml_diff>

<commit_message>
changing the day of the award dinner (had to modify the conference schedule summary in the index page, plus sigcomm program, plus social events page)
</commit_message>
<xml_diff>
--- a/docs/schedule_2016.xlsx
+++ b/docs/schedule_2016.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Calendar!$A$2:$Q$32</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Calendar!$B$2:$R$38</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
   <si>
     <t>Day</t>
   </si>
@@ -101,12 +101,6 @@
   </si>
   <si>
     <t>Tutorial 2</t>
-  </si>
-  <si>
-    <t>Workshop on Fostering Latin-American Research in Data Communication Networks</t>
-  </si>
-  <si>
-    <t>Workshop on Networking and Programming Languages</t>
   </si>
   <si>
     <t>Morning</t>
@@ -140,24 +134,9 @@
 Closing</t>
   </si>
   <si>
-    <t>Banquet</t>
-  </si>
-  <si>
     <t>Student Dinner</t>
   </si>
   <si>
-    <t>Award Dinner</t>
-  </si>
-  <si>
-    <t>Workshop on Hot Topics in Middleboxes and Network Function Virtualization</t>
-  </si>
-  <si>
-    <t>Workshop on QoE-based Analysis and Management of Data Communication Networks</t>
-  </si>
-  <si>
-    <t>Global Access to the Internet for All (GAIA) Workshop</t>
-  </si>
-  <si>
     <t>Tutorial 4</t>
   </si>
   <si>
@@ -186,11 +165,6 @@
   </si>
   <si>
     <t>Tutorial 3</t>
-  </si>
-  <si>
-    <t>Topic Preview
-Reception
-N2Women</t>
   </si>
   <si>
     <t>Late Afternoon, Evening</t>
@@ -228,7 +202,36 @@
     <t>Printing</t>
   </si>
   <si>
-    <t>200x590</t>
+    <t>Topic Preview
+Reception
+N2Women
+Award Dinner</t>
+  </si>
+  <si>
+    <t>Conference Banquet</t>
+  </si>
+  <si>
+    <t>Global Access to the Internet for All (GAIA) Workshop
+(Topazio 1)</t>
+  </si>
+  <si>
+    <t>Workshop on Hot Topics in Middleboxes and Network Function Virtualization
+(Agata 1)</t>
+  </si>
+  <si>
+    <t>Workshop on QoE-based Analysis and Management of Data Communication Networks
+(Agata 2)</t>
+  </si>
+  <si>
+    <t>Workshop on Fostering Latin-American Research in Data Communication Networks
+(Agata 1)</t>
+  </si>
+  <si>
+    <t>Workshop on Networking and Programming Languages
+(Agata 2)</t>
+  </si>
+  <si>
+    <t>200x650</t>
   </si>
 </sst>
 </file>
@@ -383,7 +386,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -850,66 +853,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -939,37 +882,13 @@
       <left style="thick">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right style="thick">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -981,25 +900,43 @@
       <right style="thick">
         <color auto="1"/>
       </right>
-      <top style="thick">
+      <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thick">
         <color auto="1"/>
       </left>
       <right style="thick">
         <color auto="1"/>
       </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -1769,7 +1706,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1801,11 +1738,42 @@
     <xf numFmtId="49" fontId="10" fillId="8" borderId="32" xfId="59" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="9" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="9" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1816,193 +1784,150 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="8" borderId="15" xfId="59" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="8" borderId="16" xfId="59" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="8" borderId="17" xfId="59" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="9" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="9" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="9" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="9" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="8" borderId="15" xfId="59" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="8" borderId="16" xfId="59" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="8" borderId="17" xfId="59" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="762">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
@@ -3105,880 +3030,992 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R68"/>
+  <dimension ref="B1:S72"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.625" style="1" customWidth="1"/>
-    <col min="3" max="15" width="16.625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="16.625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="13.625" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="11" style="2"/>
+    <col min="1" max="1" width="6.875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.625" style="1" customWidth="1"/>
+    <col min="4" max="6" width="20.625" style="2" customWidth="1"/>
+    <col min="7" max="12" width="16.625" style="2" customWidth="1"/>
+    <col min="13" max="16" width="20.625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="20.625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="13.625" style="2" customWidth="1"/>
+    <col min="19" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" thickBot="1">
-      <c r="P1" s="2"/>
-      <c r="R1" s="1"/>
-    </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="15" t="s">
+    <row r="1" spans="2:19" ht="15.75" thickBot="1">
+      <c r="Q1" s="2"/>
+      <c r="S1" s="1"/>
+    </row>
+    <row r="2" spans="2:19" s="1" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="C2" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="36" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="68"/>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="55"/>
+      <c r="I2" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="58"/>
-      <c r="J2" s="69" t="s">
+      <c r="J2" s="44"/>
+      <c r="K2" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="59"/>
-      <c r="L2" s="36" t="s">
+      <c r="L2" s="45"/>
+      <c r="M2" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="15" t="s">
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="2:19" ht="15" customHeight="1">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" ht="15" customHeight="1">
+      <c r="B4" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="36"/>
+      <c r="I4" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="40"/>
+      <c r="K4" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="49"/>
+      <c r="M4" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" ht="15" customHeight="1">
+      <c r="B5" s="18"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="61"/>
+      <c r="R5" s="18"/>
+    </row>
+    <row r="6" spans="2:19" ht="15" customHeight="1">
+      <c r="B6" s="18"/>
+      <c r="C6" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="37"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="N6" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="O6" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="P6" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="R6" s="18"/>
+    </row>
+    <row r="7" spans="2:19" ht="15" customHeight="1">
+      <c r="B7" s="18"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="61"/>
+      <c r="R7" s="18"/>
+    </row>
+    <row r="8" spans="2:19" ht="15" customHeight="1">
+      <c r="B8" s="18"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="61"/>
+      <c r="R8" s="18"/>
+    </row>
+    <row r="9" spans="2:19" ht="15" customHeight="1">
+      <c r="B9" s="18"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="40"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="18"/>
+    </row>
+    <row r="10" spans="2:19" ht="15" customHeight="1">
+      <c r="B10" s="18"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="61"/>
+      <c r="R10" s="18"/>
+    </row>
+    <row r="11" spans="2:19" ht="15" customHeight="1">
+      <c r="B11" s="18"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="61"/>
+      <c r="R11" s="18"/>
+    </row>
+    <row r="12" spans="2:19" ht="15" customHeight="1">
+      <c r="B12" s="18"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="61"/>
+      <c r="R12" s="18"/>
+    </row>
+    <row r="13" spans="2:19" ht="15" customHeight="1">
+      <c r="B13" s="18"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="61"/>
+      <c r="R13" s="18"/>
+    </row>
+    <row r="14" spans="2:19" ht="15" customHeight="1">
+      <c r="B14" s="18"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="61"/>
+      <c r="R14" s="18"/>
+    </row>
+    <row r="15" spans="2:19" ht="15" customHeight="1">
+      <c r="B15" s="18"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="63"/>
+      <c r="R15" s="18"/>
+    </row>
+    <row r="16" spans="2:19" ht="15" customHeight="1">
+      <c r="B16" s="18"/>
+      <c r="C16" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="32"/>
+      <c r="I16" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="32"/>
+      <c r="K16" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="L16" s="57"/>
+      <c r="M16" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" s="59"/>
+      <c r="O16" s="59"/>
+      <c r="P16" s="59"/>
+      <c r="Q16" s="59"/>
+      <c r="R16" s="18"/>
+    </row>
+    <row r="17" spans="2:18" ht="15" customHeight="1">
+      <c r="B17" s="18"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="59"/>
+      <c r="O17" s="59"/>
+      <c r="P17" s="59"/>
+      <c r="Q17" s="59"/>
+      <c r="R17" s="18"/>
+    </row>
+    <row r="18" spans="2:18" ht="15" customHeight="1">
+      <c r="B18" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="F18" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64" t="s">
+        <v>32</v>
+      </c>
+      <c r="L18" s="64"/>
+      <c r="M18" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="N18" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="O18" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="P18" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q18" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="R18" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" ht="15" customHeight="1">
+      <c r="B19" s="18"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="64"/>
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="61"/>
+      <c r="R19" s="18"/>
+    </row>
+    <row r="20" spans="2:18" ht="15" customHeight="1">
+      <c r="B20" s="18"/>
+      <c r="C20" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="64"/>
+      <c r="H20" s="64"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="64"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="64"/>
+      <c r="M20" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="N20" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="O20" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="P20" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q20" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="R20" s="18"/>
+    </row>
+    <row r="21" spans="2:18" ht="15" customHeight="1">
+      <c r="B21" s="18"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="61"/>
+      <c r="R21" s="18"/>
+    </row>
+    <row r="22" spans="2:18" ht="15" customHeight="1">
+      <c r="B22" s="18"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="61"/>
+      <c r="R22" s="18"/>
+    </row>
+    <row r="23" spans="2:18" ht="15" customHeight="1">
+      <c r="B23" s="18"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="61"/>
+      <c r="R23" s="18"/>
+    </row>
+    <row r="24" spans="2:18" ht="15" customHeight="1">
+      <c r="B24" s="18"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="24"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="61"/>
+      <c r="R24" s="18"/>
+    </row>
+    <row r="25" spans="2:18" ht="15" customHeight="1">
+      <c r="B25" s="18"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="64"/>
+      <c r="J25" s="64"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="61"/>
+      <c r="R25" s="18"/>
+    </row>
+    <row r="26" spans="2:18" ht="15" customHeight="1">
+      <c r="B26" s="18"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="64"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="64"/>
+      <c r="K26" s="64"/>
+      <c r="L26" s="64"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="29"/>
+      <c r="Q26" s="61"/>
+      <c r="R26" s="18"/>
+    </row>
+    <row r="27" spans="2:18" ht="15" customHeight="1">
+      <c r="B27" s="19"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="65"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="24"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="61"/>
+      <c r="R27" s="19"/>
+    </row>
+    <row r="28" spans="2:18" ht="15" customHeight="1">
+      <c r="B28" s="19"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="65"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="29"/>
+      <c r="Q28" s="61"/>
+      <c r="R28" s="19"/>
+    </row>
+    <row r="29" spans="2:18" ht="15" customHeight="1" thickBot="1">
+      <c r="B29" s="19"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="65"/>
+      <c r="I29" s="65"/>
+      <c r="J29" s="65"/>
+      <c r="K29" s="65"/>
+      <c r="L29" s="65"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="29"/>
+      <c r="Q29" s="61"/>
+      <c r="R29" s="19"/>
+    </row>
+    <row r="30" spans="2:18" ht="15" customHeight="1" thickTop="1">
+      <c r="B30" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="C30" s="68" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="H30" s="71"/>
+      <c r="I30" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30" s="74"/>
+      <c r="K30" s="77"/>
+      <c r="L30" s="77"/>
+      <c r="M30" s="77"/>
+      <c r="N30" s="77"/>
+      <c r="O30" s="77"/>
+      <c r="P30" s="77"/>
+      <c r="Q30" s="77"/>
+      <c r="R30" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="60" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q3" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="A4" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="81" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="51"/>
-      <c r="H4" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="55"/>
-      <c r="J4" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" s="63"/>
-      <c r="L4" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="N4" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="O4" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="P4" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q4" s="39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="15" customHeight="1">
-      <c r="A5" s="39"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="39"/>
-    </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1">
-      <c r="A6" s="39"/>
-      <c r="B6" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="52"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="N6" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="O6" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="P6" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q6" s="39"/>
-    </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1">
-      <c r="A7" s="39"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="39"/>
-    </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1">
-      <c r="A8" s="39"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="56"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="39"/>
-    </row>
-    <row r="9" spans="1:18" ht="15" customHeight="1">
-      <c r="A9" s="39"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="55"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="39"/>
-    </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1">
-      <c r="A10" s="39"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="39"/>
-    </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1">
-      <c r="A11" s="39"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="39"/>
-    </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1">
-      <c r="A12" s="39"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="64"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="39"/>
-    </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1">
-      <c r="A13" s="39"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="39"/>
-    </row>
-    <row r="14" spans="1:18" ht="15" customHeight="1">
-      <c r="A14" s="39"/>
-      <c r="B14" s="72" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="47"/>
-      <c r="H14" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="I14" s="47"/>
-      <c r="J14" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="K14" s="70"/>
-      <c r="L14" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="39"/>
-    </row>
-    <row r="15" spans="1:18" ht="15" customHeight="1">
-      <c r="A15" s="39"/>
-      <c r="B15" s="72"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="71"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="39"/>
-    </row>
-    <row r="16" spans="1:18" ht="15" customHeight="1">
-      <c r="A16" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="81" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16" s="20"/>
-      <c r="L16" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="M16" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="N16" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="O16" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="P16" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q16" s="39" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1">
-      <c r="A17" s="39"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="39"/>
-    </row>
-    <row r="18" spans="1:17" ht="15" customHeight="1">
-      <c r="A18" s="39"/>
-      <c r="B18" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="M18" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="N18" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="O18" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="P18" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q18" s="39"/>
-    </row>
-    <row r="19" spans="1:17" ht="15" customHeight="1">
-      <c r="A19" s="39"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="39"/>
-    </row>
-    <row r="20" spans="1:17" ht="15" customHeight="1">
-      <c r="A20" s="39"/>
-      <c r="B20" s="44"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="31"/>
-      <c r="Q20" s="39"/>
-    </row>
-    <row r="21" spans="1:17" ht="15" customHeight="1">
-      <c r="A21" s="39"/>
-      <c r="B21" s="44"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="39"/>
-    </row>
-    <row r="22" spans="1:17" ht="15" customHeight="1">
-      <c r="A22" s="39"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="31"/>
-      <c r="Q22" s="39"/>
-    </row>
-    <row r="23" spans="1:17" ht="15" customHeight="1">
-      <c r="A23" s="39"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="31"/>
-      <c r="Q23" s="39"/>
-    </row>
-    <row r="24" spans="1:17" ht="15" customHeight="1">
-      <c r="A24" s="39"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="31"/>
-      <c r="Q24" s="39"/>
-    </row>
-    <row r="25" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A25" s="39"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="45"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="43"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="32"/>
-      <c r="Q25" s="39"/>
-    </row>
-    <row r="26" spans="1:17" ht="15" customHeight="1" thickTop="1">
-      <c r="A26" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="75" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="76"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" s="21"/>
-      <c r="H26" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="I26" s="23"/>
-      <c r="J26" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="K26" s="21"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
-      <c r="P26" s="27"/>
-      <c r="Q26" s="39" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="15" customHeight="1">
-      <c r="A27" s="39"/>
-      <c r="B27" s="75"/>
-      <c r="C27" s="76"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="77"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="25"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
-      <c r="O27" s="28"/>
-      <c r="P27" s="27"/>
-      <c r="Q27" s="39"/>
-    </row>
-    <row r="28" spans="1:17" ht="15" customHeight="1">
-      <c r="A28" s="39"/>
-      <c r="B28" s="75"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="77"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
-      <c r="P28" s="27"/>
-      <c r="Q28" s="39"/>
-    </row>
-    <row r="29" spans="1:17" ht="15" customHeight="1">
-      <c r="A29" s="39"/>
-      <c r="B29" s="75"/>
-      <c r="C29" s="76"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
-      <c r="O29" s="28"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="39"/>
-    </row>
-    <row r="30" spans="1:17" ht="15" customHeight="1">
-      <c r="A30" s="39"/>
-      <c r="B30" s="75"/>
-      <c r="C30" s="76"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="77"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="28"/>
-      <c r="O30" s="28"/>
-      <c r="P30" s="27"/>
-      <c r="Q30" s="39"/>
-    </row>
-    <row r="31" spans="1:17" ht="15" customHeight="1">
-      <c r="A31" s="39"/>
-      <c r="B31" s="75"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="76"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="28"/>
-      <c r="O31" s="28"/>
-      <c r="P31" s="27"/>
-      <c r="Q31" s="39"/>
-    </row>
-    <row r="32" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A32" s="41"/>
-      <c r="B32" s="78"/>
-      <c r="C32" s="79"/>
-      <c r="D32" s="79"/>
-      <c r="E32" s="80"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="28"/>
-      <c r="N32" s="28"/>
-      <c r="O32" s="28"/>
-      <c r="P32" s="27"/>
-      <c r="Q32" s="41"/>
-    </row>
-    <row r="33" spans="18:18" ht="15" customHeight="1" thickTop="1"/>
-    <row r="34" spans="18:18" ht="15" customHeight="1"/>
-    <row r="35" spans="18:18" ht="15" customHeight="1"/>
-    <row r="36" spans="18:18" ht="15" customHeight="1"/>
-    <row r="37" spans="18:18" ht="15" customHeight="1"/>
-    <row r="38" spans="18:18" ht="15" customHeight="1"/>
-    <row r="39" spans="18:18" ht="15" customHeight="1"/>
-    <row r="40" spans="18:18" ht="15" customHeight="1"/>
-    <row r="41" spans="18:18" ht="15" customHeight="1"/>
-    <row r="42" spans="18:18" ht="15" customHeight="1"/>
-    <row r="43" spans="18:18" ht="15" customHeight="1"/>
-    <row r="44" spans="18:18" ht="15" customHeight="1"/>
-    <row r="45" spans="18:18" ht="15" customHeight="1"/>
-    <row r="46" spans="18:18" ht="15" customHeight="1"/>
-    <row r="47" spans="18:18" ht="15" customHeight="1">
-      <c r="R47" s="1"/>
-    </row>
-    <row r="48" spans="18:18" ht="15" customHeight="1">
-      <c r="R48" s="1"/>
-    </row>
-    <row r="49" spans="18:18" ht="15" customHeight="1">
-      <c r="R49" s="1"/>
-    </row>
-    <row r="50" spans="18:18" ht="15" customHeight="1"/>
-    <row r="51" spans="18:18" ht="15" customHeight="1"/>
-    <row r="52" spans="18:18" ht="15" customHeight="1"/>
-    <row r="53" spans="18:18" ht="15" customHeight="1"/>
-    <row r="54" spans="18:18" ht="15" customHeight="1"/>
-    <row r="55" spans="18:18" ht="15" customHeight="1"/>
-    <row r="56" spans="18:18" ht="15" customHeight="1"/>
-    <row r="57" spans="18:18" ht="15" customHeight="1"/>
-    <row r="58" spans="18:18" ht="15" customHeight="1"/>
-    <row r="59" spans="18:18" ht="15" customHeight="1"/>
-    <row r="60" spans="18:18" ht="15" customHeight="1"/>
-    <row r="61" spans="18:18" ht="15" customHeight="1"/>
-    <row r="62" spans="18:18" ht="15" customHeight="1"/>
-    <row r="63" spans="18:18" ht="15" customHeight="1"/>
-    <row r="64" spans="18:18" ht="15" customHeight="1"/>
+    </row>
+    <row r="31" spans="2:18" ht="15" customHeight="1">
+      <c r="B31" s="66"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="72"/>
+      <c r="H31" s="72"/>
+      <c r="I31" s="75"/>
+      <c r="J31" s="75"/>
+      <c r="K31" s="78"/>
+      <c r="L31" s="78"/>
+      <c r="M31" s="78"/>
+      <c r="N31" s="78"/>
+      <c r="O31" s="78"/>
+      <c r="P31" s="78"/>
+      <c r="Q31" s="78"/>
+      <c r="R31" s="66"/>
+    </row>
+    <row r="32" spans="2:18" ht="15" customHeight="1">
+      <c r="B32" s="66"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
+      <c r="G32" s="72"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="75"/>
+      <c r="J32" s="75"/>
+      <c r="K32" s="78"/>
+      <c r="L32" s="78"/>
+      <c r="M32" s="78"/>
+      <c r="N32" s="78"/>
+      <c r="O32" s="78"/>
+      <c r="P32" s="78"/>
+      <c r="Q32" s="78"/>
+      <c r="R32" s="66"/>
+    </row>
+    <row r="33" spans="2:18" ht="15" customHeight="1">
+      <c r="B33" s="66"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="72"/>
+      <c r="H33" s="72"/>
+      <c r="I33" s="75"/>
+      <c r="J33" s="75"/>
+      <c r="K33" s="78"/>
+      <c r="L33" s="78"/>
+      <c r="M33" s="78"/>
+      <c r="N33" s="78"/>
+      <c r="O33" s="78"/>
+      <c r="P33" s="78"/>
+      <c r="Q33" s="78"/>
+      <c r="R33" s="66"/>
+    </row>
+    <row r="34" spans="2:18" ht="15" customHeight="1">
+      <c r="B34" s="66"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="72"/>
+      <c r="H34" s="72"/>
+      <c r="I34" s="75"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="78"/>
+      <c r="L34" s="78"/>
+      <c r="M34" s="78"/>
+      <c r="N34" s="78"/>
+      <c r="O34" s="78"/>
+      <c r="P34" s="78"/>
+      <c r="Q34" s="78"/>
+      <c r="R34" s="66"/>
+    </row>
+    <row r="35" spans="2:18" ht="15" customHeight="1">
+      <c r="B35" s="66"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="72"/>
+      <c r="I35" s="75"/>
+      <c r="J35" s="75"/>
+      <c r="K35" s="78"/>
+      <c r="L35" s="78"/>
+      <c r="M35" s="78"/>
+      <c r="N35" s="78"/>
+      <c r="O35" s="78"/>
+      <c r="P35" s="78"/>
+      <c r="Q35" s="78"/>
+      <c r="R35" s="66"/>
+    </row>
+    <row r="36" spans="2:18" ht="15" customHeight="1">
+      <c r="B36" s="66"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="72"/>
+      <c r="I36" s="75"/>
+      <c r="J36" s="75"/>
+      <c r="K36" s="78"/>
+      <c r="L36" s="78"/>
+      <c r="M36" s="78"/>
+      <c r="N36" s="78"/>
+      <c r="O36" s="78"/>
+      <c r="P36" s="78"/>
+      <c r="Q36" s="78"/>
+      <c r="R36" s="66"/>
+    </row>
+    <row r="37" spans="2:18" ht="15" customHeight="1">
+      <c r="B37" s="66"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="72"/>
+      <c r="I37" s="75"/>
+      <c r="J37" s="75"/>
+      <c r="K37" s="78"/>
+      <c r="L37" s="78"/>
+      <c r="M37" s="78"/>
+      <c r="N37" s="78"/>
+      <c r="O37" s="78"/>
+      <c r="P37" s="78"/>
+      <c r="Q37" s="78"/>
+      <c r="R37" s="66"/>
+    </row>
+    <row r="38" spans="2:18" ht="15" customHeight="1" thickBot="1">
+      <c r="B38" s="67"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="70"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="73"/>
+      <c r="I38" s="76"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="78"/>
+      <c r="L38" s="78"/>
+      <c r="M38" s="78"/>
+      <c r="N38" s="78"/>
+      <c r="O38" s="78"/>
+      <c r="P38" s="78"/>
+      <c r="Q38" s="78"/>
+      <c r="R38" s="67"/>
+    </row>
+    <row r="39" spans="2:18" ht="15" customHeight="1" thickTop="1"/>
+    <row r="40" spans="2:18" ht="15" customHeight="1"/>
+    <row r="41" spans="2:18" ht="15" customHeight="1"/>
+    <row r="42" spans="2:18" ht="15" customHeight="1"/>
+    <row r="43" spans="2:18" ht="15" customHeight="1"/>
+    <row r="44" spans="2:18" ht="15" customHeight="1"/>
+    <row r="45" spans="2:18" ht="15" customHeight="1"/>
+    <row r="46" spans="2:18" ht="15" customHeight="1"/>
+    <row r="47" spans="2:18" ht="15" customHeight="1"/>
+    <row r="48" spans="2:18" ht="15" customHeight="1"/>
+    <row r="49" spans="19:19" ht="15" customHeight="1"/>
+    <row r="50" spans="19:19" ht="15" customHeight="1"/>
+    <row r="51" spans="19:19" ht="15" customHeight="1">
+      <c r="S51" s="1"/>
+    </row>
+    <row r="52" spans="19:19" ht="15" customHeight="1">
+      <c r="S52" s="1"/>
+    </row>
+    <row r="53" spans="19:19" ht="15" customHeight="1">
+      <c r="S53" s="1"/>
+    </row>
+    <row r="54" spans="19:19" ht="15" customHeight="1"/>
+    <row r="55" spans="19:19" ht="15" customHeight="1"/>
+    <row r="56" spans="19:19" ht="15" customHeight="1"/>
+    <row r="57" spans="19:19" ht="15" customHeight="1"/>
+    <row r="58" spans="19:19" ht="15" customHeight="1"/>
+    <row r="59" spans="19:19" ht="15" customHeight="1"/>
+    <row r="60" spans="19:19" ht="15" customHeight="1"/>
+    <row r="61" spans="19:19" ht="15" customHeight="1"/>
+    <row r="62" spans="19:19" ht="15" customHeight="1"/>
+    <row r="63" spans="19:19" ht="15" customHeight="1"/>
+    <row r="64" spans="19:19" ht="15" customHeight="1"/>
     <row r="65" ht="15" customHeight="1"/>
     <row r="66" ht="15" customHeight="1"/>
     <row r="67" ht="15" customHeight="1"/>
     <row r="68" ht="15" customHeight="1"/>
+    <row r="69" ht="15" customHeight="1"/>
+    <row r="70" ht="15" customHeight="1"/>
+    <row r="71" ht="15" customHeight="1"/>
+    <row r="72" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="67">
-    <mergeCell ref="A4:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A25"/>
-    <mergeCell ref="A26:A32"/>
-    <mergeCell ref="B14:E15"/>
-    <mergeCell ref="B26:E32"/>
-    <mergeCell ref="B18:B25"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="C18:C25"/>
-    <mergeCell ref="B4:B5"/>
+  <mergeCells count="66">
+    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="C30:F38"/>
+    <mergeCell ref="G30:H38"/>
+    <mergeCell ref="I30:J38"/>
+    <mergeCell ref="R30:R38"/>
+    <mergeCell ref="K30:Q38"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E29"/>
+    <mergeCell ref="K18:L29"/>
+    <mergeCell ref="G18:H29"/>
+    <mergeCell ref="I18:J29"/>
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="R4:R15"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="M6:M15"/>
+    <mergeCell ref="N6:N15"/>
+    <mergeCell ref="P6:P15"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="Q6:Q15"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="O6:O15"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="R18:R29"/>
+    <mergeCell ref="M16:Q17"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="O20:O29"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="M20:M29"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="N20:N29"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="P20:P29"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="Q20:Q29"/>
+    <mergeCell ref="G16:H17"/>
+    <mergeCell ref="G4:H8"/>
+    <mergeCell ref="G9:H15"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="I4:J15"/>
+    <mergeCell ref="K4:L15"/>
+    <mergeCell ref="C6:C15"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K16:L17"/>
+    <mergeCell ref="I16:J17"/>
+    <mergeCell ref="F6:F15"/>
+    <mergeCell ref="B4:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B29"/>
+    <mergeCell ref="C16:F17"/>
+    <mergeCell ref="C20:C29"/>
+    <mergeCell ref="D6:D15"/>
+    <mergeCell ref="D20:D29"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D6:D13"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F14:G15"/>
-    <mergeCell ref="F4:G8"/>
-    <mergeCell ref="F9:G13"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F3:K3"/>
-    <mergeCell ref="H4:I13"/>
-    <mergeCell ref="J4:K13"/>
-    <mergeCell ref="B6:B13"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J14:K15"/>
-    <mergeCell ref="H14:I15"/>
-    <mergeCell ref="E6:E13"/>
-    <mergeCell ref="Q14:Q15"/>
-    <mergeCell ref="Q16:Q25"/>
-    <mergeCell ref="Q26:Q32"/>
-    <mergeCell ref="L14:P15"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="N18:N25"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="L18:L25"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="M18:M25"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="N6:N13"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="Q4:Q13"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="L6:L13"/>
-    <mergeCell ref="M6:M13"/>
-    <mergeCell ref="O6:O13"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="P6:P13"/>
-    <mergeCell ref="F26:G32"/>
-    <mergeCell ref="H26:I32"/>
-    <mergeCell ref="J26:K32"/>
-    <mergeCell ref="L26:P32"/>
-    <mergeCell ref="F16:G25"/>
-    <mergeCell ref="H16:I25"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="O18:O25"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="P18:P25"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E18:E25"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D25"/>
-    <mergeCell ref="J16:K25"/>
+    <mergeCell ref="E6:E15"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="F20:F29"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -3996,8 +4033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4273,12 +4310,12 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="82">
+      <c r="C32" s="17">
         <v>0.95</v>
       </c>
       <c r="D32" s="6"/>

</xml_diff>